<commit_message>
Se habilita el LOGIN y se separa Celadores y Empalmadores
</commit_message>
<xml_diff>
--- a/points-managment/src/assets/PuntosTrabajadores2024.xlsx
+++ b/points-managment/src/assets/PuntosTrabajadores2024.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Mes actual" sheetId="1" r:id="rId1"/>
-    <sheet name="Historico" sheetId="2" r:id="rId2"/>
-    <sheet name="Login" sheetId="3" r:id="rId3"/>
+    <sheet name="Mes actual cel" sheetId="1" r:id="rId1"/>
+    <sheet name="Mes actual emp" sheetId="4" r:id="rId2"/>
+    <sheet name="Historico" sheetId="2" r:id="rId3"/>
+    <sheet name="Login" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Cuadrilla</t>
   </si>
@@ -29,9 +30,6 @@
     <t>Trabajador</t>
   </si>
   <si>
-    <t>Puesto</t>
-  </si>
-  <si>
     <t>Puntos</t>
   </si>
   <si>
@@ -47,23 +45,50 @@
     <t>Jose</t>
   </si>
   <si>
+    <t>BETA01</t>
+  </si>
+  <si>
+    <t>TEST01</t>
+  </si>
+  <si>
+    <t>TEST02</t>
+  </si>
+  <si>
+    <t>TEST03</t>
+  </si>
+  <si>
     <t>Casta</t>
   </si>
   <si>
-    <t>BETA01</t>
-  </si>
-  <si>
-    <t>Celador</t>
-  </si>
-  <si>
-    <t>Empalmador</t>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Psswd</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>lucas.gutierrez</t>
+  </si>
+  <si>
+    <t>HastaLosHuevos24</t>
+  </si>
+  <si>
+    <t>HastaLosHuevos25</t>
+  </si>
+  <si>
+    <t>jesus.gutierrez</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,8 +110,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,6 +128,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -123,18 +160,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bueno" xfId="2" builtinId="26"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -414,18 +460,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="8.90625" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,64 +482,71 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="C5" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1500</v>
+      <c r="C7" s="2">
+        <v>581</v>
       </c>
     </row>
   </sheetData>
@@ -502,6 +556,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -515,14 +606,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="20.36328125" customWidth="1"/>
+    <col min="3" max="3" width="22.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se acaba la generación del documento notificación cuando login
</commit_message>
<xml_diff>
--- a/points-managment/src/assets/PuntosTrabajadores2024.xlsx
+++ b/points-managment/src/assets/PuntosTrabajadores2024.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mes actual cel" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Cuadrilla</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Chus</t>
   </si>
   <si>
-    <t>Jose</t>
-  </si>
-  <si>
     <t>BETA01</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>TEST03</t>
   </si>
   <si>
-    <t>Casta</t>
-  </si>
-  <si>
     <t>Usuario</t>
   </si>
   <si>
@@ -82,6 +76,15 @@
   </si>
   <si>
     <t>jesus.gutierrez</t>
+  </si>
+  <si>
+    <t>Jesús Gutiérrez Vázquez</t>
+  </si>
+  <si>
+    <t>Jose Luis Pérez Asenjo</t>
+  </si>
+  <si>
+    <t>Christian Castaño Rodríguez</t>
   </si>
 </sst>
 </file>
@@ -463,12 +466,12 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
     <col min="3" max="3" width="8.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -487,8 +490,8 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C2" s="2">
         <v>24</v>
@@ -498,8 +501,8 @@
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C3" s="2">
         <v>658</v>
@@ -510,7 +513,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2">
         <v>78</v>
@@ -518,7 +521,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -529,10 +532,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2">
         <v>289</v>
@@ -540,10 +543,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2">
         <v>581</v>
@@ -559,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,7 +584,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2">
         <v>150</v>
@@ -610,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -622,24 +625,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -647,10 +650,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualiza código de lectura a EXCEL
</commit_message>
<xml_diff>
--- a/points-managment/src/assets/PuntosTrabajadores2024.xlsx
+++ b/points-managment/src/assets/PuntosTrabajadores2024.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Mes actual cel" sheetId="1" r:id="rId1"/>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -733,7 +733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se actualiza los puntos realizados por los trabajadores
</commit_message>
<xml_diff>
--- a/points-managment/src/assets/PuntosTrabajadores2024.xlsx
+++ b/points-managment/src/assets/PuntosTrabajadores2024.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Mes actual cel" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -195,6 +195,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bueno" xfId="2" builtinId="26"/>
@@ -479,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,7 +509,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>58.94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -519,7 +520,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>62.67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -530,7 +531,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>58.94</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -576,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,8 +604,8 @@
       <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2">
-        <v>0</v>
+      <c r="C2" s="7">
+        <v>84.168800000000005</v>
       </c>
     </row>
   </sheetData>
@@ -616,7 +617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se redondea a dos decimales los putnos restantes
</commit_message>
<xml_diff>
--- a/points-managment/src/assets/PuntosTrabajadores2024.xlsx
+++ b/points-managment/src/assets/PuntosTrabajadores2024.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mes actual cel" sheetId="1" r:id="rId1"/>
@@ -480,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,7 +605,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="7">
-        <v>84.168800000000005</v>
+        <v>84.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualiza puntos trabajadores
</commit_message>
<xml_diff>
--- a/points-managment/src/assets/PuntosTrabajadores2024.xlsx
+++ b/points-managment/src/assets/PuntosTrabajadores2024.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="25">
   <si>
     <t>Cuadrilla</t>
   </si>
@@ -481,7 +481,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -509,7 +509,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="2">
-        <v>63.265000000000001</v>
+        <v>63.865000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -520,7 +520,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="2">
-        <v>63.265000000000001</v>
+        <v>63.865000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -531,7 +531,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="2">
-        <v>63.265000000000001</v>
+        <v>63.865000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -578,7 +578,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,7 +605,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="7">
-        <v>84.16</v>
+        <v>141.88999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualiza puntos de los trabajadores
</commit_message>
<xml_diff>
--- a/points-managment/src/assets/PuntosTrabajadores2024.xlsx
+++ b/points-managment/src/assets/PuntosTrabajadores2024.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
   <si>
     <t>Cuadrilla</t>
   </si>
@@ -481,7 +481,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -509,7 +509,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="2">
-        <v>63.865000000000002</v>
+        <v>74.155000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -578,7 +578,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,7 +605,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="7">
-        <v>141.88999999999999</v>
+        <v>160.05000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se incrementa el número de puntos
</commit_message>
<xml_diff>
--- a/points-managment/src/assets/PuntosTrabajadores2024.xlsx
+++ b/points-managment/src/assets/PuntosTrabajadores2024.xlsx
@@ -581,7 +581,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -608,7 +608,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="7">
-        <v>38.81</v>
+        <v>117.13720000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>